<commit_message>
Adding base html, css and js files
</commit_message>
<xml_diff>
--- a/data/gamer stat percentages by country, age, gender/hours_per_week_by_country.xlsx
+++ b/data/gamer stat percentages by country, age, gender/hours_per_week_by_country.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcbie\RICE_BOOTCAMP\Working Folder\Project_Two\Project-2\data\gamer stat percentages by country\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcbie\RICE_BOOTCAMP\Working Folder\Project_Two\Project-2\data\gamer stat percentages by country, age, gender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0881EA91-CF2E-4009-9E08-5D2367A58D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7ABFC0-B550-44E2-B60B-635BBAAA2884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{100434AC-E4E9-4759-8909-5AFC1781627A}"/>
+    <workbookView xWindow="2490" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{100434AC-E4E9-4759-8909-5AFC1781627A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>More than 20 hours per week</t>
   </si>
   <si>
-    <t>Average Hoiurs Each Week</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Global</t>
+  </si>
+  <si>
+    <t>Average Hours Each Week</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BC9ED5-5C22-48C0-8CB2-2064A8DA9CD1}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -482,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -540,7 +542,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>0.152</v>
@@ -581,7 +583,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>0.108</v>
@@ -622,7 +624,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>0.13</v>
@@ -663,7 +665,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>0.21199999999999999</v>
@@ -704,7 +706,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>0.14799999999999999</v>
@@ -745,7 +747,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>0.17799999999999999</v>
@@ -786,7 +788,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>0.154</v>
@@ -827,7 +829,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>0.128</v>
@@ -868,7 +870,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>0.14899999999999999</v>

</xml_diff>